<commit_message>
add Error type FrozenSimulationError that's raised by an SSA submodel when it is the only submodel and total propensities == 0; ensure that DynamicRateLaws get made if RateLaw(s) exist; replace rate law evaluation with dynamic rate law evaluation; fix initialization of SSASubmodel & more comprehensively test it; in DynamicSubmodel use DynamicReactions and DynamicRateLaws, add some optimizations and planning comments
</commit_message>
<xml_diff>
--- a/tests/multialgorithm/fixtures/validation/cases/stochastic/00030/00030-wc_lang.xlsx
+++ b/tests/multialgorithm/fixtures/validation/cases/stochastic/00030/00030-wc_lang.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-27720" yWindow="2560" windowWidth="27220" windowHeight="9160" tabRatio="500" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="940" yWindow="460" windowWidth="23720" windowHeight="5680" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Model" sheetId="1" r:id="rId1"/>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="88">
   <si>
     <t>Id</t>
   </si>
@@ -323,7 +323,10 @@
     <t>k2</t>
   </si>
   <si>
-    <t>Volume matters in reactions that aren't order 1</t>
+    <t>Mass balance the reactions</t>
+  </si>
+  <si>
+    <t>Volume matters in reactions that aren't order 1; V(0) = 1/NA</t>
   </si>
 </sst>
 </file>
@@ -333,7 +336,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000E+00"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -371,6 +374,11 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Menlo"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -401,7 +409,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -431,6 +439,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1"/>
+    <xf numFmtId="11" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Explanatory Text" xfId="1" builtinId="53" customBuiltin="1"/>
@@ -782,8 +791,8 @@
   <sheetPr codeName="Sheet1" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView zoomScale="133" zoomScaleNormal="133" zoomScalePageLayoutView="133" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1454,7 +1463,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="133" zoomScaleNormal="133" zoomScalePageLayoutView="133" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1462,7 +1471,7 @@
     <col min="1" max="1" width="5.1640625" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.1640625" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.1640625" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.5" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="33.5" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.5" style="2" customWidth="1"/>
@@ -1501,12 +1510,12 @@
       <c r="C2" t="s">
         <v>75</v>
       </c>
-      <c r="D2" s="4">
-        <v>1</v>
+      <c r="D2" s="13">
+        <v>1.6605390404271598E-24</v>
       </c>
       <c r="E2" s="4"/>
       <c r="F2" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -1522,7 +1531,7 @@
   <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView zoomScale="133" zoomScaleNormal="133" zoomScalePageLayoutView="133" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1590,7 +1599,9 @@
       <c r="H2" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="I2" s="5"/>
+      <c r="I2" s="5" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
@@ -1604,7 +1615,7 @@
       </c>
       <c r="D3"/>
       <c r="F3" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G3" s="2">
         <v>0</v>
@@ -1626,7 +1637,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView zoomScale="133" zoomScaleNormal="133" zoomScalePageLayoutView="133" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1735,9 +1746,7 @@
   <sheetPr codeName="Sheet8" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:E1"/>
   <sheetViews>
-    <sheetView zoomScale="133" zoomScaleNormal="133" zoomScalePageLayoutView="133" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView zoomScale="133" zoomScaleNormal="133" zoomScalePageLayoutView="133" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>

</xml_diff>